<commit_message>
update api add search think by bilijeans
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\一哥\Desktop\manga-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11881F83-5C25-4295-A40B-EF78B8088C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8C6748-A5F3-4FFC-8D44-DFBEAC71C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>排行榜</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -291,6 +291,25 @@
   </si>
   <si>
     <t>https://hw-chapter2.51kanmanhua.com/comic/C/%E7%A9%BF%E8%B6%8A%E8%A5%BF%E5%85%833000%E5%90%8E/%E7%AC%AC8%E8%AF%9DF2_131939/1.jpg-kmh.middle?auth_key=1664797469-994cca4f51aa42d9a683480ce077a1b8-0-002d629d3c9b8867b988c5e726738348</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>漫画搜索联想</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.kanman.com/api/getsortlist</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>search_key</t>
+  </si>
+  <si>
+    <t>搜索关键字</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你好</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -301,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,16 +371,31 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -369,6 +403,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -376,28 +490,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,7 +504,46 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -414,13 +552,55 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -704,628 +884,723 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="X59" sqref="X59"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="14.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="65.625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="14.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="65.625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="15" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15">
         <v>0</v>
       </c>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="11" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="11" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="11" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="11" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="11" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="11" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="11" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="11" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="11" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="15">
         <v>1</v>
       </c>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="15">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-    </row>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="7"/>
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="11" t="s">
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="7"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="6"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="7"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="7"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="6"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="11"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="7"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="7"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="6"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="15">
         <v>1</v>
       </c>
-      <c r="F37" s="11"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="15">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="2" t="s">
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
+      <c r="B39" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="33" t="s">
         <v>53</v>
       </c>
-    </row>
+      <c r="F39" s="24"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="15">
         <v>5754</v>
       </c>
-      <c r="F44" s="11"/>
+      <c r="F44" s="32"/>
     </row>
     <row r="45" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="2" t="s">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="15">
         <v>8009</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="2" t="s">
+      <c r="F45" s="16"/>
+    </row>
+    <row r="46" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="22"/>
+      <c r="B46" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="D46" s="23"/>
+      <c r="E46" s="33" t="s">
         <v>68</v>
       </c>
-    </row>
+      <c r="F46" s="24"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13"/>
     </row>
     <row r="50" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="25"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="24"/>
+    </row>
+    <row r="52" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-    </row>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="27"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
+    </row>
+    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="10"/>
+    </row>
+    <row r="62" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="37"/>
+    </row>
+    <row r="63" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" s="30"/>
+    </row>
+    <row r="64" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="E65" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="C6:C15"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:F43"/>
     <mergeCell ref="B54:F54"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="A57:F57"/>
@@ -1335,23 +1610,6 @@
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="C6:C15"/>
-    <mergeCell ref="A3:A18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add rank view by bilijeans
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\一哥\Desktop\manga-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8C6748-A5F3-4FFC-8D44-DFBEAC71C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3700104-2CED-4C45-BB90-A8774E94FD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,57 +72,30 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>综合</t>
   </si>
   <si>
-    <t>Self</t>
-  </si>
-  <si>
     <t>自制</t>
   </si>
   <si>
-    <t>Boy</t>
-  </si>
-  <si>
     <t>男生</t>
   </si>
   <si>
-    <t>Girl</t>
-  </si>
-  <si>
     <t>女生</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
     <t>新作</t>
   </si>
   <si>
-    <t>Dark</t>
-  </si>
-  <si>
     <t>黑马</t>
   </si>
   <si>
-    <t>Charge</t>
-  </si>
-  <si>
     <t>付费</t>
   </si>
   <si>
-    <t>Free</t>
-  </si>
-  <si>
     <t>免费</t>
   </si>
   <si>
-    <t>Finish</t>
-  </si>
-  <si>
     <t>完结</t>
   </si>
   <si>
@@ -310,6 +283,42 @@
   </si>
   <si>
     <t>你好</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>boy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>girl</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>new</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>charge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>free</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -320,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +387,14 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -484,13 +501,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,44 +531,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -567,22 +552,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -597,15 +573,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
     <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -886,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:M22"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -900,259 +904,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="16"/>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="19" t="s">
+      <c r="E7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="19" t="s">
+      <c r="E9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="19" t="s">
+      <c r="E11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="19" t="s">
+      <c r="E13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="19" t="s">
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="19" t="s">
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28"/>
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="20" t="s">
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="15">
-        <v>1</v>
-      </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="E17" s="1">
         <v>100</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
+      <c r="A20" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="27"/>
+      <c r="B21" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -1162,41 +1164,41 @@
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
+      <c r="B25" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="30" t="s">
-        <v>42</v>
+      <c r="B26" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1221,44 +1223,44 @@
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
+      <c r="A30" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
+      <c r="B31" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="23" t="s">
+      <c r="B32" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" s="30"/>
+      <c r="D32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
@@ -1275,303 +1277,303 @@
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
+      <c r="A35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
+      <c r="B36" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="15" t="s">
+      <c r="B37" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="15">
+      <c r="D37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="1">
         <v>1</v>
       </c>
-      <c r="F37" s="32"/>
+      <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="15" t="s">
+      <c r="A38" s="28"/>
+      <c r="B38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" s="15">
+      <c r="D38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="1">
         <v>12</v>
       </c>
-      <c r="F38" s="16"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="23" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="24"/>
+      <c r="D39" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="13"/>
     </row>
     <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10"/>
+      <c r="A42" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="24"/>
     </row>
     <row r="43" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
+      <c r="B43" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="15" t="s">
+      <c r="B44" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="1">
+        <v>5754</v>
+      </c>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="28"/>
+      <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="15">
-        <v>5754</v>
-      </c>
-      <c r="F44" s="32"/>
-    </row>
-    <row r="45" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" s="15">
+      <c r="D45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="1">
         <v>8009</v>
       </c>
-      <c r="F45" s="16"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="23" t="s">
+      <c r="A46" s="29"/>
+      <c r="B46" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F46" s="24"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="10"/>
+      <c r="A48" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="24"/>
     </row>
     <row r="49" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="13"/>
+      <c r="B49" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="13"/>
+      <c r="A50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26"/>
     </row>
     <row r="51" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="24"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="10"/>
+      <c r="A53" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="13"/>
+      <c r="B54" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="26"/>
     </row>
     <row r="55" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="27"/>
+      <c r="B55" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="31"/>
     </row>
     <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="10"/>
+      <c r="A57" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="24"/>
     </row>
     <row r="58" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="13"/>
+      <c r="B58" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="26"/>
     </row>
     <row r="59" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="35"/>
+      <c r="A59" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="21"/>
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="10"/>
+      <c r="A61" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="24"/>
     </row>
     <row r="62" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="37"/>
+      <c r="B62" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="26"/>
     </row>
     <row r="63" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="23" t="s">
+      <c r="B63" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="F63" s="30"/>
+      <c r="D63" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F63" s="16"/>
     </row>
     <row r="64" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
@@ -1582,6 +1584,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="A30:F30"/>
@@ -1598,20 +1612,11 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="B36:F36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="A53:F53"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C26" r:id="rId1" xr:uid="{C73C049E-C529-4468-8F2C-257A41BDF62E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add rely on route and integration code by bilijeans
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\桌面\y\Project\manga-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\一哥\Desktop\manga-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9526120F-9C39-439E-B9A3-A44701DAD450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E40D7D-6597-43FA-9464-150F56A23E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="83">
   <si>
     <t>排行榜</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -330,6 +330,14 @@
   </si>
   <si>
     <t>heat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>漫画目录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.kanman.com/api/getchapterlist</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -340,7 +348,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,7 +527,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -539,9 +547,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -584,43 +589,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -905,22 +910,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:E26"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="14.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="65.58203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="14.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="65.625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="37.5" customHeight="1">
+    <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -930,11 +935,11 @@
       <c r="E1" s="23"/>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="25"/>
@@ -942,8 +947,8 @@
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -958,10 +963,10 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A4" s="27"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -971,10 +976,10 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A5" s="27"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -984,11 +989,11 @@
       <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="31" t="s">
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
+      <c r="B6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -1000,11 +1005,11 @@
       <c r="E6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="31"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="25"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
@@ -1012,11 +1017,11 @@
       <c r="E7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="31"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="25"/>
       <c r="D8" s="5" t="s">
         <v>14</v>
@@ -1024,11 +1029,11 @@
       <c r="E8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A9" s="27"/>
-      <c r="B9" s="31"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="25"/>
       <c r="D9" s="5" t="s">
         <v>15</v>
@@ -1036,11 +1041,11 @@
       <c r="E9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="31"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="25"/>
       <c r="D10" s="5" t="s">
         <v>16</v>
@@ -1048,11 +1053,11 @@
       <c r="E10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="31"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="25"/>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -1060,11 +1065,11 @@
       <c r="E11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A12" s="27"/>
-      <c r="B12" s="31"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="25"/>
       <c r="D12" s="5" t="s">
         <v>18</v>
@@ -1072,11 +1077,11 @@
       <c r="E12" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A13" s="27"/>
-      <c r="B13" s="31"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="25"/>
       <c r="D13" s="5" t="s">
         <v>19</v>
@@ -1084,11 +1089,11 @@
       <c r="E13" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="31"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="25"/>
       <c r="D14" s="5" t="s">
         <v>20</v>
@@ -1096,11 +1101,11 @@
       <c r="E14" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="31"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="25"/>
       <c r="D15" s="5" t="s">
         <v>22</v>
@@ -1108,10 +1113,10 @@
       <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A16" s="27"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1124,10 +1129,10 @@
       <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A17" s="27"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
       <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1140,24 +1145,24 @@
       <c r="E17" s="1">
         <v>100</v>
       </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A18" s="28"/>
-      <c r="B18" s="12" t="s">
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" ht="14.5" thickBot="1"/>
-    <row r="20" spans="1:6" ht="25.5" customHeight="1">
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>28</v>
       </c>
@@ -1167,26 +1172,26 @@
       <c r="E20" s="23"/>
       <c r="F20" s="24"/>
     </row>
-    <row r="21" spans="1:6" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="25.5" customHeight="1" thickBot="1">
+    <row r="23" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="25.5" customHeight="1">
+    <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>29</v>
       </c>
@@ -1196,11 +1201,11 @@
       <c r="E24" s="23"/>
       <c r="F24" s="24"/>
     </row>
-    <row r="25" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="25"/>
@@ -1208,44 +1213,44 @@
       <c r="E25" s="25"/>
       <c r="F25" s="26"/>
     </row>
-    <row r="26" spans="1:6" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="16" t="s">
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" customHeight="1">
+    <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="25.5" customHeight="1">
+    <row r="28" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="14.5" thickBot="1">
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="25.5" customHeight="1">
+    <row r="30" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>34</v>
       </c>
@@ -1255,8 +1260,8 @@
       <c r="E30" s="23"/>
       <c r="F30" s="24"/>
     </row>
-    <row r="31" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="25" t="s">
@@ -1267,39 +1272,39 @@
       <c r="E31" s="25"/>
       <c r="F31" s="26"/>
     </row>
-    <row r="32" spans="1:6" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="1:6" ht="25.5" customHeight="1">
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="25.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="25.5" customHeight="1">
+    <row r="35" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>40</v>
       </c>
@@ -1309,11 +1314,11 @@
       <c r="E35" s="23"/>
       <c r="F35" s="24"/>
     </row>
-    <row r="36" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="27" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="25"/>
@@ -1321,11 +1326,11 @@
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A37" s="27" t="s">
+    <row r="37" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1337,10 +1342,10 @@
       <c r="E37" s="1">
         <v>1</v>
       </c>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A38" s="27"/>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="29"/>
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -1353,26 +1358,26 @@
       <c r="E38" s="1">
         <v>12</v>
       </c>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A39" s="28"/>
-      <c r="B39" s="12" t="s">
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="13"/>
-    </row>
-    <row r="41" spans="1:6" ht="14.5" thickBot="1"/>
-    <row r="42" spans="1:6" ht="25.5" customHeight="1">
+      <c r="F39" s="12"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>45</v>
       </c>
@@ -1382,8 +1387,8 @@
       <c r="E42" s="23"/>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="25" t="s">
@@ -1394,11 +1399,11 @@
       <c r="E43" s="25"/>
       <c r="F43" s="26"/>
     </row>
-    <row r="44" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A44" s="27" t="s">
+    <row r="44" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1410,10 +1415,10 @@
       <c r="E44" s="1">
         <v>5754</v>
       </c>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A45" s="27"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="29"/>
       <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1426,24 +1431,24 @@
       <c r="E45" s="1">
         <v>8009</v>
       </c>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A46" s="28"/>
-      <c r="B46" s="12" t="s">
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+      <c r="B46" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="19" t="s">
+      <c r="D46" s="11"/>
+      <c r="E46" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:6" ht="14.5" thickBot="1"/>
-    <row r="48" spans="1:6" ht="26.25" customHeight="1">
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>49</v>
       </c>
@@ -1453,8 +1458,8 @@
       <c r="E48" s="23"/>
       <c r="F48" s="24"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B49" s="25" t="s">
@@ -1465,8 +1470,8 @@
       <c r="E49" s="25"/>
       <c r="F49" s="26"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1479,16 +1484,16 @@
       <c r="E50" s="25"/>
       <c r="F50" s="26"/>
     </row>
-    <row r="51" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A51" s="14"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:6" ht="26.25" customHeight="1" thickBot="1"/>
-    <row r="53" spans="1:6" ht="26.25" customHeight="1">
+    <row r="51" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
         <v>54</v>
       </c>
@@ -1498,11 +1503,11 @@
       <c r="E53" s="23"/>
       <c r="F53" s="24"/>
     </row>
-    <row r="54" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A54" s="8" t="s">
+    <row r="54" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="27" t="s">
         <v>55</v>
       </c>
       <c r="C54" s="25"/>
@@ -1510,20 +1515,20 @@
       <c r="E54" s="25"/>
       <c r="F54" s="26"/>
     </row>
-    <row r="55" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="30"/>
-    </row>
-    <row r="56" spans="1:6" ht="14.5" thickBot="1"/>
-    <row r="57" spans="1:6" ht="26.25" customHeight="1">
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
         <v>57</v>
       </c>
@@ -1533,8 +1538,8 @@
       <c r="E57" s="23"/>
       <c r="F57" s="24"/>
     </row>
-    <row r="58" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A58" s="8" t="s">
+    <row r="58" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="25" t="s">
@@ -1545,20 +1550,20 @@
       <c r="E58" s="25"/>
       <c r="F58" s="26"/>
     </row>
-    <row r="59" spans="1:6" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A59" s="14" t="s">
+    <row r="59" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="21"/>
-    </row>
-    <row r="60" spans="1:6" ht="14.5" thickBot="1"/>
-    <row r="61" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="20"/>
+    </row>
+    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
         <v>64</v>
       </c>
@@ -1568,8 +1573,8 @@
       <c r="E61" s="23"/>
       <c r="F61" s="24"/>
     </row>
-    <row r="62" spans="1:6" ht="27.75" customHeight="1">
-      <c r="A62" s="8" t="s">
+    <row r="62" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="25" t="s">
@@ -1580,33 +1585,83 @@
       <c r="E62" s="25"/>
       <c r="F62" s="26"/>
     </row>
-    <row r="63" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A63" s="11" t="s">
+    <row r="63" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="12" t="s">
+      <c r="D63" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F63" s="16"/>
-    </row>
-    <row r="64" spans="1:6" ht="27.75" customHeight="1">
+      <c r="F63" s="15"/>
+    </row>
+    <row r="64" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
     </row>
-    <row r="65" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A65" s="4"/>
-      <c r="E65" s="7"/>
+    <row r="65" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="24"/>
+    </row>
+    <row r="66" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="26"/>
+    </row>
+    <row r="67" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="11">
+        <v>106619</v>
+      </c>
+      <c r="F67" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="30">
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="A30:F30"/>
@@ -1623,18 +1678,6 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="B36:F36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="A53:F53"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1644,8 +1687,9 @@
     <hyperlink ref="B2" r:id="rId4" xr:uid="{EB3F835F-6F38-4BFC-9FA0-0FD07F3522FC}"/>
     <hyperlink ref="B54" r:id="rId5" xr:uid="{C1E4C963-7282-4C10-A020-C4F1169B5976}"/>
     <hyperlink ref="B25" r:id="rId6" xr:uid="{83670FA2-CB98-486A-84E3-1EA5C589E6EB}"/>
+    <hyperlink ref="B66" r:id="rId7" xr:uid="{2CC1113C-24CD-4460-AC1E-60AF5B589ACC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add readView and readTools,create localStorage for bookcase by bilijeans
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\一哥\Desktop\manga-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E40D7D-6597-43FA-9464-150F56A23E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD00F54-82AC-4BFB-BB20-D0848C18E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -601,28 +601,28 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:F66"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -939,16 +939,16 @@
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -966,7 +966,7 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -979,7 +979,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -992,11 +992,11 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="26" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -1008,9 +1008,9 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="25"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1020,9 +1020,9 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1032,9 +1032,9 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
@@ -1044,9 +1044,9 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1056,9 +1056,9 @@
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="25"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1068,9 +1068,9 @@
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1080,9 +1080,9 @@
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1092,9 +1092,9 @@
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
@@ -1104,9 +1104,9 @@
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="25"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="11" t="s">
         <v>78</v>
       </c>
@@ -1176,13 +1176,13 @@
       <c r="A21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -1205,13 +1205,13 @@
       <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1223,8 +1223,8 @@
       <c r="C26" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="15" t="s">
         <v>33</v>
       </c>
@@ -1264,13 +1264,13 @@
       <c r="A31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
@@ -1318,16 +1318,16 @@
       <c r="A36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
     </row>
     <row r="37" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="16" t="s">
@@ -1345,7 +1345,7 @@
       <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="11" t="s">
         <v>42</v>
       </c>
@@ -1391,16 +1391,16 @@
       <c r="A43" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="27"/>
     </row>
     <row r="44" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="16" t="s">
@@ -1418,7 +1418,7 @@
       <c r="F44" s="17"/>
     </row>
     <row r="45" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="11" t="s">
         <v>58</v>
       </c>
@@ -1465,10 +1465,10 @@
       <c r="B49" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="27"/>
     </row>
     <row r="50" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
@@ -1477,12 +1477,12 @@
       <c r="B50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="27"/>
     </row>
     <row r="51" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
@@ -1507,25 +1507,25 @@
       <c r="A54" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="27"/>
     </row>
     <row r="55" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="32"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="31"/>
     </row>
     <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1542,13 +1542,13 @@
       <c r="A58" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="27"/>
     </row>
     <row r="59" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
@@ -1577,13 +1577,13 @@
       <c r="A62" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="27"/>
     </row>
     <row r="63" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
@@ -1620,13 +1620,13 @@
       <c r="A66" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="27" t="s">
+      <c r="B66" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="27"/>
     </row>
     <row r="67" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
@@ -1648,22 +1648,8 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="B36:F36"/>
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="A1:F1"/>
@@ -1676,8 +1662,22 @@
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="B62:F62"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1688,8 +1688,9 @@
     <hyperlink ref="B54" r:id="rId5" xr:uid="{C1E4C963-7282-4C10-A020-C4F1169B5976}"/>
     <hyperlink ref="B25" r:id="rId6" xr:uid="{83670FA2-CB98-486A-84E3-1EA5C589E6EB}"/>
     <hyperlink ref="B66" r:id="rId7" xr:uid="{2CC1113C-24CD-4460-AC1E-60AF5B589ACC}"/>
+    <hyperlink ref="B49" r:id="rId8" xr:uid="{EE0271B7-CC58-4E96-A04C-6342DD8AC9FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add searchResultView and deal with some bug by bilijeans
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\一哥\Desktop\manga-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD00F54-82AC-4BFB-BB20-D0848C18E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F0B364-24B1-46FA-9E22-EE1EE1314888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,6 +610,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -620,9 +623,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -948,7 +948,7 @@
       <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -966,7 +966,7 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -979,7 +979,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -992,8 +992,8 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="32" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -1008,8 +1008,8 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="26"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
@@ -1020,8 +1020,8 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="26"/>
       <c r="D8" s="5" t="s">
         <v>14</v>
@@ -1032,8 +1032,8 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="26"/>
       <c r="D9" s="5" t="s">
         <v>15</v>
@@ -1044,8 +1044,8 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="26"/>
       <c r="D10" s="5" t="s">
         <v>16</v>
@@ -1056,8 +1056,8 @@
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="26"/>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -1068,8 +1068,8 @@
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="26"/>
       <c r="D12" s="5" t="s">
         <v>18</v>
@@ -1080,8 +1080,8 @@
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="26"/>
       <c r="D13" s="5" t="s">
         <v>19</v>
@@ -1092,8 +1092,8 @@
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="26"/>
       <c r="D14" s="5" t="s">
         <v>20</v>
@@ -1104,8 +1104,8 @@
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="26"/>
       <c r="D15" s="5" t="s">
         <v>22</v>
@@ -1116,7 +1116,7 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="11" t="s">
         <v>78</v>
       </c>
@@ -1176,13 +1176,13 @@
       <c r="A21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -1223,8 +1223,8 @@
       <c r="C26" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="15" t="s">
         <v>33</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="F36" s="27"/>
     </row>
     <row r="37" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="16" t="s">
@@ -1345,7 +1345,7 @@
       <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="11" t="s">
         <v>42</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="F43" s="27"/>
     </row>
     <row r="44" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="16" t="s">
@@ -1418,7 +1418,7 @@
       <c r="F44" s="17"/>
     </row>
     <row r="45" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="28"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="11" t="s">
         <v>58</v>
       </c>
@@ -1519,13 +1519,13 @@
       <c r="A55" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
     </row>
     <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1648,6 +1648,22 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="A30:F30"/>
@@ -1662,22 +1678,6 @@
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="B62:F62"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1689,8 +1689,9 @@
     <hyperlink ref="B25" r:id="rId6" xr:uid="{83670FA2-CB98-486A-84E3-1EA5C589E6EB}"/>
     <hyperlink ref="B66" r:id="rId7" xr:uid="{2CC1113C-24CD-4460-AC1E-60AF5B589ACC}"/>
     <hyperlink ref="B49" r:id="rId8" xr:uid="{EE0271B7-CC58-4E96-A04C-6342DD8AC9FC}"/>
+    <hyperlink ref="B21" r:id="rId9" xr:uid="{288BED0F-CF7D-437D-A554-26D2C7F7A553}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>